<commit_message>
plan de riesgos, y lanzamiento TSP
nuevas actualizaciones tipo ACME
</commit_message>
<xml_diff>
--- a/3CM1_IS_T15_ACME.xlsx
+++ b/3CM1_IS_T15_ACME.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leoboyean\Documents\GitHub\AcmeDev\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-165" yWindow="15" windowWidth="15600" windowHeight="7620" tabRatio="869"/>
   </bookViews>
   <sheets>
     <sheet name="Riesgos" sheetId="30" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -118,61 +123,61 @@
     <t>Describa las actividades dirigidas a evitar que el riesgo se dispare. Incluya claramente cómos y cuándos.</t>
   </si>
   <si>
-    <t>No terminar el proyecto a tiempo</t>
-  </si>
-  <si>
-    <t>Intentar terminar las tareas a tiempo</t>
-  </si>
-  <si>
     <t>A, T, M, J</t>
   </si>
   <si>
-    <t xml:space="preserve">Riesgo de no aprender a tiempo sobre aplicaciones móviles y no poder desarrollar los juegos </t>
-  </si>
-  <si>
-    <t>Aprender android extraclase</t>
-  </si>
-  <si>
-    <t>No poder manipular correctamente los gráficos</t>
-  </si>
-  <si>
     <t>No terminar el proyecto completo(la parte de web)</t>
   </si>
   <si>
-    <t>No terminar el proyecto completo(la parte de moviles)</t>
-  </si>
-  <si>
-    <t>Aprender desarrollo de aplicaciones web extraclase</t>
-  </si>
-  <si>
-    <t>Una vez disipado este riesgo no se podrá terminar a tiempo el proyecto</t>
-  </si>
-  <si>
-    <t>Una vez disipado este riesgo no se podrá terminar ningún juego móvil a tiempo y se tendrá que postergar la entrega de este.</t>
-  </si>
-  <si>
-    <t>Una vez disipado este riesgo no se podrá terminar ningún juego web a tiempo y se tendrá que entregar la entrega de este.</t>
-  </si>
-  <si>
-    <t>El riesgo de las tareas con dependencia, no poder continuar porque alguien no ha hecho una tarea que se necesita para realizar otra</t>
-  </si>
-  <si>
-    <t>Se retrasarán el avances de las tareas y podría haber un desfase</t>
-  </si>
-  <si>
-    <t>El riesgo que puede pasar más posiblemente es el desfase de tiempo, pues ahora queda menos tiempo para realizar las tareas restantes</t>
-  </si>
-  <si>
-    <t>Dar prioridad a las tareas con dependencia</t>
-  </si>
-  <si>
-    <t>Realizar tareas de las cuales se depende lo más pronto posible, para seguir con la tarea que se debe de realizar después.</t>
-  </si>
-  <si>
     <t>Equipo ACME:  Joel, Teodoro, Maricela y Alan</t>
   </si>
   <si>
     <t>3CM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No adquirir la capasitación necesaria para el desarrollo de aplicaciónes móviles </t>
+  </si>
+  <si>
+    <t>Desfase de tiempo para terminar el proyecto(la parte de moviles)</t>
+  </si>
+  <si>
+    <t>Aprender lo mas amplio posible del manejo de android en horas extraclase</t>
+  </si>
+  <si>
+    <t>Se tendrá que posponer la fecha de entrega.</t>
+  </si>
+  <si>
+    <t>No saber manipular correctamente los gráficos en la web.</t>
+  </si>
+  <si>
+    <t>Aprender a desarrollar aplicaciones web en horas extraclase.</t>
+  </si>
+  <si>
+    <t>No se podrá terminar ningún juego web.</t>
+  </si>
+  <si>
+    <t>Alguna de las tareas que tienen dependencia no sea terminada en el tiempo planeado.</t>
+  </si>
+  <si>
+    <t>Se retrasarán los avances de nuevas tareas.</t>
+  </si>
+  <si>
+    <t>Dar prioridad a las tareas con dependencia.</t>
+  </si>
+  <si>
+    <t>Finalizar la tareas lo más pronto posible, para continuar con la tarea que se debe de realizar después.</t>
+  </si>
+  <si>
+    <t>Nuestro cliente no acepte los prototipos</t>
+  </si>
+  <si>
+    <t>Desfase de tiempo para rediseñarlos.</t>
+  </si>
+  <si>
+    <t>Hacer que los prototipos cumplan con la mayoría de los requisitos propuestos por el cliente.</t>
+  </si>
+  <si>
+    <t>Volver a hacer nuevos prototipos.</t>
   </si>
 </sst>
 </file>
@@ -620,7 +625,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -732,6 +737,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1214,7 +1222,7 @@
   <dimension ref="B1:P28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1348,7 +1356,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B5" s="9">
         <f>B4+1</f>
         <v>1</v>
@@ -1357,10 +1365,10 @@
         <v>42015</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>5</v>
@@ -1369,16 +1377,16 @@
         <v>6</v>
       </c>
       <c r="H5" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M5" s="8" t="s">
         <v>2</v>
@@ -1393,7 +1401,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="9">
         <f t="shared" ref="B6:B24" si="0">B5+1</f>
         <v>2</v>
@@ -1402,10 +1410,10 @@
         <v>42015</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F6" s="15" t="s">
         <v>5</v>
@@ -1414,16 +1422,16 @@
         <v>6</v>
       </c>
       <c r="H6" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>44</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>14</v>
@@ -1443,10 +1451,10 @@
         <v>42015</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>5</v>
@@ -1455,16 +1463,16 @@
         <v>6</v>
       </c>
       <c r="H7" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
@@ -1473,7 +1481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B8" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1481,29 +1489,29 @@
       <c r="C8" s="21">
         <v>42015</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="15" t="s">
+      <c r="D8" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>6</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="17">
+        <v>7</v>
+      </c>
+      <c r="H8" s="16">
         <v>1</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>49</v>
+      <c r="I8" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
@@ -1796,12 +1804,12 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D27" s="12" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D28" s="12" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NO CE QUE PEDO, PLAN DE RIESGOS
LOL ES LO MISMO
</commit_message>
<xml_diff>
--- a/3CM1_IS_T15_ACME.xlsx
+++ b/3CM1_IS_T15_ACME.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leoboyean\Documents\GitHub\AcmeDev\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-165" yWindow="15" windowWidth="15600" windowHeight="7620" tabRatio="869"/>
   </bookViews>
   <sheets>
     <sheet name="Riesgos" sheetId="30" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>Aceptado</t>
   </si>
@@ -130,6 +135,9 @@
     <t>3CM1</t>
   </si>
   <si>
+    <t xml:space="preserve">No adquirir la capasitación necesaria para el desarrollo de aplicaciónes móviles </t>
+  </si>
+  <si>
     <t>Desfase de tiempo para terminar el proyecto(la parte de moviles)</t>
   </si>
   <si>
@@ -160,7 +168,16 @@
     <t>Finalizar la tareas lo más pronto posible, para continuar con la tarea que se debe de realizar después.</t>
   </si>
   <si>
-    <t xml:space="preserve">No adquirir la capacitación necesaria para el desarrollo de aplicaciónes móviles </t>
+    <t>Nuestro cliente no acepte los prototipos</t>
+  </si>
+  <si>
+    <t>Desfase de tiempo para rediseñarlos.</t>
+  </si>
+  <si>
+    <t>Hacer que los prototipos cumplan con la mayoría de los requisitos propuestos por el cliente.</t>
+  </si>
+  <si>
+    <t>Volver a hacer nuevos prototipos.</t>
   </si>
 </sst>
 </file>
@@ -706,23 +723,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1205,7 +1222,7 @@
   <dimension ref="B1:P28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:K8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1229,22 +1246,22 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" s="1" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="35" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="34"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="33" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="34"/>
-      <c r="K2" s="37"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="36"/>
       <c r="L2" s="13"/>
       <c r="M2" s="14" t="s">
         <v>9</v>
@@ -1348,10 +1365,10 @@
         <v>42015</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>5</v>
@@ -1363,10 +1380,10 @@
         <v>1</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>34</v>
@@ -1393,7 +1410,7 @@
         <v>42015</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>35</v>
@@ -1408,10 +1425,10 @@
         <v>2</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>34</v>
@@ -1434,10 +1451,10 @@
         <v>42015</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>5</v>
@@ -1449,10 +1466,10 @@
         <v>1</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>34</v>
@@ -1464,19 +1481,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B8" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="3"/>
+      <c r="C8" s="21">
+        <v>42015</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="16">
+        <v>1</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="9">

</xml_diff>